<commit_message>
transformation functionality added (#11)
* transformation functionality added

* Update ghga_transpiler/config/config.py

---------

Co-authored-by: Leon Kuchenbecker <leon.kuchenbecker@uni-tuebingen.de>
</commit_message>
<xml_diff>
--- a/tests/fixtures/workbooks/a_workbook.xlsx
+++ b/tests/fixtures/workbooks/a_workbook.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/dev/ghga-transpiler/tests/fixtures/workbooks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bilgesurun/Desktop/dev/ghga-transpiler/tests/fixtures/workbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAEE9999-069C-4647-8276-4AC72B530638}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94621525-EAFF-9944-AE73-F8A24DF37D17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3300" yWindow="3740" windowWidth="28800" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3300" yWindow="3740" windowWidth="28800" windowHeight="16100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="__properties" sheetId="16" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>writer_name</t>
   </si>
@@ -58,12 +58,6 @@
     <t>Secker and Warburg</t>
   </si>
   <si>
-    <t>publisher_name</t>
-  </si>
-  <si>
-    <t>Hamish Hamilton</t>
-  </si>
-  <si>
     <t>9783548234106</t>
   </si>
   <si>
@@ -74,6 +68,18 @@
   </si>
   <si>
     <t>0.0.0</t>
+  </si>
+  <si>
+    <t>attributes</t>
+  </si>
+  <si>
+    <t>page = 100; cover= paperback</t>
+  </si>
+  <si>
+    <t>Hamish Hamilton; Stephen King</t>
+  </si>
+  <si>
+    <t>publisher_names</t>
   </si>
 </sst>
 </file>
@@ -343,7 +349,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{678FC2E7-48D1-8A4E-B11A-27CA8959732D}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -351,7 +357,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -364,7 +370,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -394,7 +400,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
@@ -402,10 +408,10 @@
         <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -415,36 +421,44 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56614A42-2C55-A544-9FE8-0C1F3BCFEB4C}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="4" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A3" s="3" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A3" s="3" t="s">
-        <v>9</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>6</v>
@@ -452,5 +466,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
tests added for the conversion plur stringcase lib
</commit_message>
<xml_diff>
--- a/tests/fixtures/workbooks/a_workbook.xlsx
+++ b/tests/fixtures/workbooks/a_workbook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bilgesurun/Desktop/dev/ghga-transpiler/tests/fixtures/workbooks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/dev/ghga-transpiler/tests/fixtures/workbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94621525-EAFF-9944-AE73-F8A24DF37D17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA669C62-E88B-9045-9712-220EAF6BA4EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3300" yWindow="3740" windowWidth="28800" windowHeight="16100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3300" yWindow="3740" windowWidth="42360" windowHeight="22280" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="__properties" sheetId="16" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>writer_name</t>
   </si>
@@ -80,6 +80,24 @@
   </si>
   <si>
     <t>publisher_names</t>
+  </si>
+  <si>
+    <t>genre</t>
+  </si>
+  <si>
+    <t>Philosophical novel; absurdist novel</t>
+  </si>
+  <si>
+    <t>dystopian novel;cautionary tale</t>
+  </si>
+  <si>
+    <t>set_in</t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>French Algeria</t>
   </si>
 </sst>
 </file>
@@ -367,10 +385,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31EA5899-C9FA-1942-A6F2-92F5BCB75FA2}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -381,7 +399,7 @@
     <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -391,8 +409,14 @@
       <c r="C1" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -402,8 +426,14 @@
       <c r="C2" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -412,6 +442,12 @@
       </c>
       <c r="C3" s="3" t="s">
         <v>7</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -423,14 +459,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56614A42-2C55-A544-9FE8-0C1F3BCFEB4C}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="2" max="2" width="28" customWidth="1"/>
     <col min="3" max="4" width="27" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Task/convert cv uppercase (#28)
* template update

* dependency update

* cv SNAKE_CASE conversion

* Version Bump

* Fix package name

---------

Co-authored-by: Léon Kuchenbecker <leon.kuchenbecker@uni-tuebingen.de>
</commit_message>
<xml_diff>
--- a/tests/fixtures/workbooks/a_workbook.xlsx
+++ b/tests/fixtures/workbooks/a_workbook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bilgesurun/Desktop/dev/ghga-transpiler/tests/fixtures/workbooks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/dev/ghga-transpiler/tests/fixtures/workbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94621525-EAFF-9944-AE73-F8A24DF37D17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA669C62-E88B-9045-9712-220EAF6BA4EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3300" yWindow="3740" windowWidth="28800" windowHeight="16100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3300" yWindow="3740" windowWidth="42360" windowHeight="22280" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="__properties" sheetId="16" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>writer_name</t>
   </si>
@@ -80,6 +80,24 @@
   </si>
   <si>
     <t>publisher_names</t>
+  </si>
+  <si>
+    <t>genre</t>
+  </si>
+  <si>
+    <t>Philosophical novel; absurdist novel</t>
+  </si>
+  <si>
+    <t>dystopian novel;cautionary tale</t>
+  </si>
+  <si>
+    <t>set_in</t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>French Algeria</t>
   </si>
 </sst>
 </file>
@@ -367,10 +385,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31EA5899-C9FA-1942-A6F2-92F5BCB75FA2}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -381,7 +399,7 @@
     <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -391,8 +409,14 @@
       <c r="C1" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -402,8 +426,14 @@
       <c r="C2" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="D2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -412,6 +442,12 @@
       </c>
       <c r="C3" s="3" t="s">
         <v>7</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -423,14 +459,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56614A42-2C55-A544-9FE8-0C1F3BCFEB4C}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="2" max="2" width="28" customWidth="1"/>
     <col min="3" max="4" width="27" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
datapack tests and functions
</commit_message>
<xml_diff>
--- a/tests/fixtures/workbooks/a_workbook.xlsx
+++ b/tests/fixtures/workbooks/a_workbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/dev/ghga-transpiler/tests/fixtures/workbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DA9D5E8-36C4-3740-9E2B-0F561049F901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C78B45FD-0EE9-E942-B582-ACF18E4B6916}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3300" yWindow="3740" windowWidth="42360" windowHeight="22280" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3300" yWindow="3740" windowWidth="42360" windowHeight="22280" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="__transpiler_protocol" sheetId="16" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="37">
   <si>
     <t>writer_name</t>
   </si>
@@ -145,6 +145,9 @@
   </si>
   <si>
     <t>object</t>
+  </si>
+  <si>
+    <t>primary_key</t>
   </si>
 </sst>
 </file>
@@ -432,15 +435,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914FC978-6391-AA4C-A042-6CE9C2BCBA1F}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -453,8 +456,11 @@
       <c r="D1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E1" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>25</v>
       </c>
@@ -467,8 +473,11 @@
       <c r="D2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E2" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>26</v>
       </c>
@@ -480,6 +489,9 @@
       </c>
       <c r="D3">
         <v>2</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -491,8 +503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7A9A923-2A75-FC4E-BE59-4B97CEBD4F7A}">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
parser and models implementation
</commit_message>
<xml_diff>
--- a/tests/fixtures/workbooks/a_workbook.xlsx
+++ b/tests/fixtures/workbooks/a_workbook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/dev/ghga-transpiler/tests/fixtures/workbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DA9D5E8-36C4-3740-9E2B-0F561049F901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E843B21D-131E-7F45-9455-F1238167C43C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3300" yWindow="3740" windowWidth="42360" windowHeight="22280" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28800" yWindow="5720" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="__transpiler_protocol" sheetId="16" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="37">
   <si>
     <t>writer_name</t>
   </si>
@@ -145,6 +145,9 @@
   </si>
   <si>
     <t>object</t>
+  </si>
+  <si>
+    <t>primary_key</t>
   </si>
 </sst>
 </file>
@@ -432,15 +435,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914FC978-6391-AA4C-A042-6CE9C2BCBA1F}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -453,8 +456,11 @@
       <c r="D1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E1" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>25</v>
       </c>
@@ -467,8 +473,11 @@
       <c r="D2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E2" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>26</v>
       </c>
@@ -480,6 +489,9 @@
       </c>
       <c r="D3">
         <v>2</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -491,7 +503,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7A9A923-2A75-FC4E-BE59-4B97CEBD4F7A}">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -703,9 +715,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31EA5899-C9FA-1942-A6F2-92F5BCB75FA2}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -775,9 +785,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56614A42-2C55-A544-9FE8-0C1F3BCFEB4C}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>

</xml_diff>

<commit_message>
schemapack adjustments in transpiler (#51)
* transpiler refactoring

* template update

* removed package compatibility for older python versions



---------

Co-authored-by: Leon Kuchenbecker <leon.kuchenbecker@uni-tuebingen.de>
Co-authored-by: Christoph Zwerschke <c.zwerschke@dkfz-heidelberg.de>
</commit_message>
<xml_diff>
--- a/tests/fixtures/workbooks/a_workbook.xlsx
+++ b/tests/fixtures/workbooks/a_workbook.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/dev/ghga-transpiler/tests/fixtures/workbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA669C62-E88B-9045-9712-220EAF6BA4EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E843B21D-131E-7F45-9455-F1238167C43C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3300" yWindow="3740" windowWidth="42360" windowHeight="22280" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28800" yWindow="5720" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="__properties" sheetId="16" r:id="rId1"/>
-    <sheet name="books" sheetId="17" r:id="rId2"/>
-    <sheet name="publisher" sheetId="18" r:id="rId3"/>
+    <sheet name="__transpiler_protocol" sheetId="16" r:id="rId1"/>
+    <sheet name="__sheet_meta" sheetId="19" r:id="rId2"/>
+    <sheet name="__column_meta" sheetId="20" r:id="rId3"/>
+    <sheet name="books" sheetId="17" r:id="rId4"/>
+    <sheet name="publisher" sheetId="18" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="37">
   <si>
     <t>writer_name</t>
   </si>
@@ -98,6 +100,54 @@
   </si>
   <si>
     <t>French Algeria</t>
+  </si>
+  <si>
+    <t>sheet</t>
+  </si>
+  <si>
+    <t>n_cols</t>
+  </si>
+  <si>
+    <t>header_row</t>
+  </si>
+  <si>
+    <t>data_start</t>
+  </si>
+  <si>
+    <t>books</t>
+  </si>
+  <si>
+    <t>publisher</t>
+  </si>
+  <si>
+    <t>column</t>
+  </si>
+  <si>
+    <t>multivalued</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>ref_class</t>
+  </si>
+  <si>
+    <t>ref_class_id_property</t>
+  </si>
+  <si>
+    <t>enum</t>
+  </si>
+  <si>
+    <t>required</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>object</t>
+  </si>
+  <si>
+    <t>primary_key</t>
   </si>
 </sst>
 </file>
@@ -368,7 +418,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -384,12 +434,288 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914FC978-6391-AA4C-A042-6CE9C2BCBA1F}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7A9A923-2A75-FC4E-BE59-4B97CEBD4F7A}">
+  <dimension ref="A1:H41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" t="b">
+        <v>0</v>
+      </c>
+      <c r="H9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="3:5" x14ac:dyDescent="0.15">
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31EA5899-C9FA-1942-A6F2-92F5BCB75FA2}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -455,13 +781,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56614A42-2C55-A544-9FE8-0C1F3BCFEB4C}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>

</xml_diff>

<commit_message>
template and schemapack update
</commit_message>
<xml_diff>
--- a/tests/fixtures/workbooks/a_workbook.xlsx
+++ b/tests/fixtures/workbooks/a_workbook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/dev/ghga-transpiler/tests/fixtures/workbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E843B21D-131E-7F45-9455-F1238167C43C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20062C60-4308-A847-B910-0868500BACA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="5720" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15700" yWindow="4700" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="__transpiler_protocol" sheetId="16" r:id="rId1"/>
@@ -437,7 +437,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{914FC978-6391-AA4C-A042-6CE9C2BCBA1F}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -503,8 +503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7A9A923-2A75-FC4E-BE59-4B97CEBD4F7A}">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -588,6 +588,12 @@
       <c r="D4" s="2" t="s">
         <v>34</v>
       </c>
+      <c r="E4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="G4" t="b">
         <v>0</v>
       </c>
@@ -648,12 +654,8 @@
       <c r="D7" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
       <c r="G7" t="b">
         <v>0</v>
       </c>

</xml_diff>